<commit_message>
Made changes in scripts
</commit_message>
<xml_diff>
--- a/Extra_Prac/Store_Creation/TestData/Store_Data.xlsx
+++ b/Extra_Prac/Store_Creation/TestData/Store_Data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -62,13 +62,16 @@
     <t xml:space="preserve">markup_type</t>
   </si>
   <si>
+    <t xml:space="preserve">markup_master</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flat_markup</t>
+  </si>
+  <si>
     <t xml:space="preserve">pay_on_account</t>
   </si>
   <si>
-    <t xml:space="preserve">markup_master</t>
-  </si>
-  <si>
-    <t xml:space="preserve">flat_markup</t>
+    <t xml:space="preserve">pay_on_limit</t>
   </si>
   <si>
     <t xml:space="preserve">open_b2b_store</t>
@@ -83,12 +86,24 @@
     <t xml:space="preserve">fix_shipping_address</t>
   </si>
   <si>
+    <t xml:space="preserve">order_approval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">show_price_to_customer</t>
+  </si>
+  <si>
     <t xml:space="preserve">quick_checkout</t>
   </si>
   <si>
+    <t xml:space="preserve">store_fields</t>
+  </si>
+  <si>
     <t xml:space="preserve">allow_tax_exemption</t>
   </si>
   <si>
+    <t xml:space="preserve">manage_invoice</t>
+  </si>
+  <si>
     <t xml:space="preserve">allow_partial_payment</t>
   </si>
   <si>
@@ -128,6 +143,15 @@
     <t xml:space="preserve">Custom</t>
   </si>
   <si>
+    <t xml:space="preserve">Store wise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both</t>
+  </si>
+  <si>
     <t xml:space="preserve">10Prints</t>
   </si>
   <si>
@@ -155,6 +179,18 @@
     <t xml:space="preserve">Finesse</t>
   </si>
   <si>
+    <t xml:space="preserve">Disable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Order wise only</t>
+  </si>
+  <si>
     <t xml:space="preserve">11Prints</t>
   </si>
   <si>
@@ -174,6 +210,18 @@
   </si>
   <si>
     <t xml:space="preserve">Crystals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer wise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partial Order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mandatory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stores</t>
   </si>
 </sst>
 </file>
@@ -292,7 +340,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="C4 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -329,10 +377,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:AB4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P6" activeCellId="0" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -374,13 +422,13 @@
       <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="0" t="s">
         <v>13</v>
       </c>
       <c r="M1" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="O1" s="0" t="s">
@@ -409,212 +457,278 @@
       </c>
       <c r="W1" s="0" t="s">
         <v>24</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>8789878978</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="J2" s="3" t="n">
         <v>1</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="N2" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="N2" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="O2" s="0" t="n">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="P2" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" s="0" t="n">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="U2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="V2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="W2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>8789878979</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J3" s="3" t="n">
         <v>0</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="N3" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="N3" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="O3" s="0" t="n">
-        <v>1</v>
+        <v>250000</v>
       </c>
       <c r="P3" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R3" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="T3" s="0" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="U3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="V3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="X3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>8789878980</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="J4" s="3" t="n">
         <v>1</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="N4" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="M4" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="N4" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="O4" s="0" t="n">
-        <v>0</v>
+        <v>500000</v>
       </c>
       <c r="P4" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T4" s="0" t="n">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="T4" s="0" t="s">
+        <v>64</v>
       </c>
       <c r="U4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="V4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="W4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="X4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="0" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>